<commit_message>
Resolved a Mistake in the Number of Hosts Sheet and updated screenshot in PPT as well
</commit_message>
<xml_diff>
--- a/Subnetting-Slides/Subnetting-Demo.xlsx
+++ b/Subnetting-Slides/Subnetting-Demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohan\Downloads\Subnetting-WB\Subnetting-Slides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4F5C0D-9484-403E-A4F9-FCB6AFCF207A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3CCF33-AE02-45AE-A219-AC51BFFF888D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="8" activeTab="11" xr2:uid="{B18EFC63-7084-4254-936D-1CF15B67B537}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{B18EFC63-7084-4254-936D-1CF15B67B537}"/>
   </bookViews>
   <sheets>
     <sheet name="IP-Table" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,24 @@
     <sheet name="# of Hosts" sheetId="8" r:id="rId8"/>
     <sheet name="NW_Broadcast" sheetId="9" r:id="rId9"/>
     <sheet name="CIDR" sheetId="10" r:id="rId10"/>
-    <sheet name="Classful_Vs_Classless_IPs" sheetId="11" r:id="rId11"/>
+    <sheet name="Classful_IPs" sheetId="11" r:id="rId11"/>
     <sheet name="Private-IP-Addresses" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -668,19 +679,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -696,7 +700,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,137 +718,139 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,9 +870,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -905,7 +910,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1011,7 +1016,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1153,7 +1158,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1161,7 +1166,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1C69D1-763D-4CBA-9F2A-1DECBACDEB7A}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G5"/>
@@ -1179,159 +1184,157 @@
     <col min="8" max="8" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+    </row>
+    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="6">
         <v>1</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="6">
         <v>3</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>2</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="6">
         <v>65000</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>3</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="6">
         <v>254</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="10" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="10" t="s">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1357,95 +1360,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="34" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="35" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="35" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="35" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="57"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="60"/>
+      <c r="C5" s="36"/>
     </row>
     <row r="6" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="34" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="35" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="35" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="35" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1481,70 +1482,70 @@
       <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="35" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="62">
+      <c r="C3" s="38">
         <v>16777214</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="35" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="62">
+      <c r="C4" s="38">
         <v>65534</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="35" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="35">
         <v>254</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="35" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1560,7 +1561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A969788-3832-48B8-9AE1-A46A12EAA26F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1571,42 +1572,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="37" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="35" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="35" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="40" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="40" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1630,66 +1631,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="6" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1714,82 +1715,82 @@
   <sheetData>
     <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="12">
+      <c r="B4" s="8">
         <v>0</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="12">
+      <c r="B5" s="8">
         <v>128</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="12">
+      <c r="B6" s="8">
         <v>192</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="12">
+      <c r="B7" s="8">
         <v>224</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="12">
+      <c r="B8" s="8">
         <v>240</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="12">
+      <c r="B9" s="8">
         <v>248</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="12">
+      <c r="B10" s="8">
         <v>252</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12">
+      <c r="B11" s="8">
         <v>254</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12">
+      <c r="B12" s="8">
         <v>255</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1810,54 +1811,54 @@
   <sheetData>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12">
+      <c r="A5" s="8">
         <v>128</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="8">
         <v>64</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="8">
         <v>32</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="8">
         <v>16</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="8">
         <v>8</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="8">
         <v>4</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="8">
         <v>2</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="8">
         <v>1</v>
       </c>
     </row>
@@ -1905,20 +1906,20 @@
       <c r="B5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="14"/>
+      <c r="E5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="10"/>
       <c r="G5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -1929,107 +1930,107 @@
       <c r="A7" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="17" t="s">
+      <c r="E7" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="17" t="s">
+      <c r="H7" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="G8" s="16" t="s">
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="G8" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="C11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="15">
+      <c r="E11" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="11">
         <v>1111</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H11" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" s="22" t="s">
+      <c r="H11" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="24" t="s">
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2063,79 +2064,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="24" t="s">
         <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="46" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="24" t="s">
         <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="10" t="s">
         <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -2143,97 +2144,97 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="26" t="s">
+      <c r="E9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="26" t="s">
+      <c r="G9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="F10" s="40" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="F10" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="C11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="18" t="s">
         <v>70</v>
       </c>
       <c r="F11" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="H11" s="26" t="s">
+      <c r="G11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A13:I13"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A13:I13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2254,82 +2255,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="24" t="s">
         <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="46" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="24" t="s">
         <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="42" t="s">
+      <c r="E7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>86</v>
       </c>
       <c r="G7" s="1">
         <v>1111</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -2337,119 +2338,119 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" s="32" t="s">
+      <c r="C9" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="29">
+      <c r="E9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="19">
         <v>1111</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="I9" s="26" t="s">
+      <c r="H9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="36"/>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="40" t="s">
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="C11" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="41" t="s">
+      <c r="E11" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="H11" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="I11" s="26" t="s">
+      <c r="H11" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
     </row>
     <row r="14" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A13:I14"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A4:H4"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A13:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2459,8 +2460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAEF5A08-C709-4E9F-82F9-F4D3996B6F54}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2472,93 +2473,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="47">
+      <c r="F1" s="54">
         <f>2^16</f>
         <v>65536</v>
       </c>
-      <c r="G1" s="46">
+      <c r="G1" s="53">
         <v>-2</v>
       </c>
-      <c r="H1" s="47">
+      <c r="H1" s="54">
         <f>F1-2</f>
         <v>65534</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="47"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="19" t="s">
+      <c r="C4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="17" t="s">
+      <c r="E4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="17" t="s">
+      <c r="G4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="F5" s="16" t="s">
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="F5" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="29" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2566,87 +2567,96 @@
       <c r="A10" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="C10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="15">
+      <c r="E10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" s="11">
         <v>1111</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="22" t="s">
+      <c r="H10" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="24" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="54" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="46" t="s">
+      <c r="E13" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="F13" s="47">
+      <c r="F13" s="54">
         <f>2^12</f>
         <v>4096</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="53">
         <v>-2</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H13" s="54">
         <f>F13-2</f>
         <v>4094</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47"/>
+      <c r="A14" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="B13:B14"/>
@@ -2656,15 +2666,6 @@
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2674,7 +2675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25928F-88DF-43DB-B839-DF93B64BF756}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A43" sqref="A43:I43"/>
     </sheetView>
   </sheetViews>
@@ -2712,20 +2713,20 @@
       <c r="B3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="14"/>
+      <c r="E3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="10"/>
       <c r="G3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -2736,49 +2737,49 @@
       <c r="A5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="17" t="s">
+      <c r="E5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="G6" s="16" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="G6" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G8" s="51" t="s">
+      <c r="G8" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -2787,20 +2788,20 @@
       <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F9" s="14"/>
+      <c r="E9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="10"/>
       <c r="G9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -2808,26 +2809,26 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -2836,20 +2837,20 @@
       <c r="B12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="14"/>
+      <c r="E12" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="10"/>
       <c r="G12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -2857,17 +2858,17 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -2890,22 +2891,22 @@
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="37" t="s">
+      <c r="E18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="25" t="s">
         <v>86</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I18" s="1" t="s">
@@ -2913,69 +2914,69 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="19" t="s">
+      <c r="C21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="15">
+      <c r="E21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="11">
         <v>1111</v>
       </c>
-      <c r="G21" s="50" t="s">
+      <c r="G21" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="22" t="s">
+      <c r="H21" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="24" t="s">
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G24" s="51" t="s">
+      <c r="G24" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -2984,22 +2985,22 @@
       <c r="B25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="37" t="s">
+      <c r="E25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="37" t="s">
+      <c r="G25" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -3007,26 +3008,26 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="51" t="s">
+      <c r="A26" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="51"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G27" s="52" t="s">
+      <c r="G27" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -3035,22 +3036,22 @@
       <c r="B28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="37" t="s">
+      <c r="E28" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="25" t="s">
         <v>86</v>
       </c>
       <c r="G28" s="1">
         <v>1111</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -3058,17 +3059,17 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -3096,22 +3097,22 @@
       <c r="B35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F35" s="38" t="s">
+      <c r="E35" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="G35" s="38" t="s">
+      <c r="G35" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -3125,22 +3126,22 @@
       <c r="B36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="10" t="s">
         <v>70</v>
       </c>
       <c r="F36" s="1">
         <v>1111</v>
       </c>
-      <c r="G36" s="38" t="s">
+      <c r="G36" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -3148,27 +3149,27 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="55" t="s">
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G38" s="51" t="s">
+      <c r="G38" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="51"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="59"/>
+      <c r="J38" s="59"/>
+      <c r="K38" s="59"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -3177,22 +3178,22 @@
       <c r="B39" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F39" s="38" t="s">
+      <c r="E39" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F39" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="H39" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -3200,26 +3201,26 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="51" t="s">
+      <c r="A40" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
+      <c r="B40" s="59"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="59"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="G41" s="52" t="s">
+      <c r="G41" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="60"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -3228,22 +3229,22 @@
       <c r="B42" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F42" s="38" t="s">
+      <c r="E42" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F42" s="26" t="s">
         <v>105</v>
       </c>
       <c r="G42" s="1">
         <v>1111</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="10" t="s">
         <v>70</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -3251,27 +3252,20 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="55"/>
+      <c r="G43" s="55"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="A29:I29"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G38:K38"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="G41:K41"/>
     <mergeCell ref="G24:K24"/>
     <mergeCell ref="A26:I26"/>
     <mergeCell ref="G27:K27"/>
@@ -3284,6 +3278,13 @@
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="A13:I13"/>
+    <mergeCell ref="A43:I43"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G38:K38"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="G41:K41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>